<commit_message>
September 8 Commit all. Too many updates to detail.
</commit_message>
<xml_diff>
--- a/SchedulerData/Configuration File.xlsx
+++ b/SchedulerData/Configuration File.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\MathnasiumScheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonPrograms\Scheduler\SchedulerData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9244D0CD-8566-42FD-90B8-D6809A943A49}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20475" windowHeight="6885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,11 +16,12 @@
     <sheet name="Config.Stafford" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="62">
   <si>
     <t>Instructor</t>
   </si>
@@ -27,36 +29,6 @@
     <t>Rank</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Max/Wk</t>
-  </si>
-  <si>
-    <t>Min/Day</t>
-  </si>
-  <si>
-    <t>Rank: Sun</t>
-  </si>
-  <si>
-    <t>Rank: Mon</t>
-  </si>
-  <si>
-    <t>Rank: Tue</t>
-  </si>
-  <si>
-    <t>Rank: Wed</t>
-  </si>
-  <si>
-    <t>Rank: Thu</t>
-  </si>
-  <si>
-    <t>Rank: Fri</t>
-  </si>
-  <si>
-    <t>Rank: Sat</t>
-  </si>
-  <si>
     <t>Availability</t>
   </si>
   <si>
@@ -69,12 +41,6 @@
     <t>Alyssah Marshall</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Sachin Sharad</t>
   </si>
   <si>
@@ -93,9 +59,6 @@
     <t>Bryant Ricks</t>
   </si>
   <si>
-    <t>Andrew Misdary</t>
-  </si>
-  <si>
     <t>Tyler Danzig</t>
   </si>
   <si>
@@ -108,30 +71,6 @@
     <t>Olivia Evans</t>
   </si>
   <si>
-    <t>Gap 1</t>
-  </si>
-  <si>
-    <t>Gap 2</t>
-  </si>
-  <si>
-    <t>Gap 3</t>
-  </si>
-  <si>
-    <t>Gap 4</t>
-  </si>
-  <si>
-    <t>Gap 5</t>
-  </si>
-  <si>
-    <t>Gap 6</t>
-  </si>
-  <si>
-    <t>Gap 7</t>
-  </si>
-  <si>
-    <t>Gap 8</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -141,9 +80,6 @@
     <t>collisonaishaha@gmail.com</t>
   </si>
   <si>
-    <t>andrewmi2000@gmail.com</t>
-  </si>
-  <si>
     <t>andygreco23@gmail.com</t>
   </si>
   <si>
@@ -199,6 +135,78 @@
   </si>
   <si>
     <t>Richard Higginbotham</t>
+  </si>
+  <si>
+    <t>Cassie Hudson</t>
+  </si>
+  <si>
+    <t>cassiemae52@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jacob Zimmerman</t>
+  </si>
+  <si>
+    <t>jzimmerman710@gmail.com</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Roland Agorkle</t>
+  </si>
+  <si>
+    <t>rkagorkle1@yahoo.com</t>
+  </si>
+  <si>
+    <t>Preferance 1</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Perference 2</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Preferance 2</t>
+  </si>
+  <si>
+    <t>Perference 3</t>
+  </si>
+  <si>
+    <t>Preferance 3</t>
+  </si>
+  <si>
+    <t>Perference 4</t>
+  </si>
+  <si>
+    <t>Preferance 4</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Max Hrs/Wk</t>
+  </si>
+  <si>
+    <t>Min Hrs/Day</t>
+  </si>
+  <si>
+    <t>Cost/Hr</t>
   </si>
 </sst>
 </file>
@@ -341,12 +349,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -646,7 +652,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -689,13 +695,12 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -729,7 +734,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1050,75 +1054,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A8" sqref="A8:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="O1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
+      <c r="Q1" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -1132,43 +1150,43 @@
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2">
-        <v>99</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>99</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" t="s">
+        <v>58</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>29230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1182,46 +1200,46 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>99</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>99</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" t="s">
+        <v>58</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>29249</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -1232,46 +1250,50 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4">
-        <v>99</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>99</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" t="s">
+        <v>58</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>59452</v>
+      </c>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
         <v>16</v>
-      </c>
-      <c r="P4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5">
-        <v>14</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -1282,46 +1304,46 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5">
-        <v>99</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>99</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" t="s">
+        <v>58</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>29254</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>15</v>
@@ -1332,46 +1354,49 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6">
-        <v>99</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>99</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" t="s">
+        <v>58</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P6" t="s">
-        <v>17</v>
+        <v>4</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>29211</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>15</v>
@@ -1382,46 +1407,46 @@
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7">
-        <v>99</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>99</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" t="s">
+        <v>58</v>
       </c>
       <c r="N7">
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>17</v>
-      </c>
-      <c r="P7" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>29210</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>15</v>
@@ -1432,46 +1457,46 @@
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="G8">
-        <v>99</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>99</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" t="s">
+        <v>58</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>29226</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>15</v>
@@ -1482,46 +1507,46 @@
       <c r="F9">
         <v>2</v>
       </c>
-      <c r="G9">
-        <v>99</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>99</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" t="s">
+        <v>58</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>17</v>
-      </c>
-      <c r="P9" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>29256</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -1532,46 +1557,46 @@
       <c r="F10">
         <v>2</v>
       </c>
-      <c r="G10">
-        <v>99</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>99</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" t="s">
+        <v>58</v>
       </c>
       <c r="N10">
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>17</v>
-      </c>
-      <c r="P10" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>29221</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <v>15</v>
@@ -1582,46 +1607,49 @@
       <c r="F11">
         <v>2</v>
       </c>
-      <c r="G11">
-        <v>99</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>99</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" t="s">
+        <v>57</v>
+      </c>
+      <c r="M11" t="s">
+        <v>58</v>
       </c>
       <c r="N11">
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P11" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>29212</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C12">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>15</v>
@@ -1632,46 +1660,46 @@
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="G12">
-        <v>99</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>99</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M12" t="s">
+        <v>58</v>
       </c>
       <c r="N12">
         <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>17</v>
-      </c>
-      <c r="P12" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>29213</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C13">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>15</v>
@@ -1682,46 +1710,46 @@
       <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13">
-        <v>99</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>99</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13" t="s">
+        <v>57</v>
+      </c>
+      <c r="M13" t="s">
+        <v>58</v>
       </c>
       <c r="N13">
         <v>1</v>
       </c>
       <c r="O13" t="s">
-        <v>17</v>
-      </c>
-      <c r="P13" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>29243</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <v>15</v>
@@ -1732,46 +1760,46 @@
       <c r="F14">
         <v>2</v>
       </c>
-      <c r="G14">
-        <v>99</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>99</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" t="s">
+        <v>57</v>
+      </c>
+      <c r="M14" t="s">
+        <v>58</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>17</v>
-      </c>
-      <c r="P14" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>29231</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C15">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="D15">
         <v>15</v>
@@ -1782,46 +1810,46 @@
       <c r="F15">
         <v>2</v>
       </c>
-      <c r="G15">
-        <v>99</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>99</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" t="s">
+        <v>58</v>
       </c>
       <c r="N15">
         <v>1</v>
       </c>
       <c r="O15" t="s">
-        <v>17</v>
-      </c>
-      <c r="P15" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>29227</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C16">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -1832,46 +1860,46 @@
       <c r="F16">
         <v>2</v>
       </c>
-      <c r="G16">
-        <v>99</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>99</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" t="s">
+        <v>57</v>
+      </c>
+      <c r="M16" t="s">
+        <v>58</v>
       </c>
       <c r="N16">
         <v>1</v>
       </c>
       <c r="O16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>29225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
         <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17">
-        <v>15</v>
       </c>
       <c r="D17">
         <v>15</v>
@@ -1882,46 +1910,46 @@
       <c r="F17">
         <v>2</v>
       </c>
-      <c r="G17">
-        <v>99</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>99</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" t="s">
+        <v>57</v>
+      </c>
+      <c r="M17" t="s">
+        <v>58</v>
       </c>
       <c r="N17">
         <v>1</v>
       </c>
       <c r="O17" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P17" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>15</v>
@@ -1932,46 +1960,49 @@
       <c r="F18">
         <v>2</v>
       </c>
-      <c r="G18">
-        <v>99</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>99</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" t="s">
+        <v>57</v>
+      </c>
+      <c r="M18" t="s">
+        <v>58</v>
       </c>
       <c r="N18">
         <v>1</v>
       </c>
       <c r="O18" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P18" t="s">
-        <v>17</v>
+        <v>4</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>63404</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <v>15</v>
@@ -1982,46 +2013,46 @@
       <c r="F19">
         <v>2</v>
       </c>
-      <c r="G19">
-        <v>99</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>99</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" t="s">
+        <v>56</v>
+      </c>
+      <c r="L19" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19" t="s">
+        <v>58</v>
       </c>
       <c r="N19">
         <v>1</v>
       </c>
       <c r="O19" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P19" t="s">
-        <v>17</v>
+        <v>4</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>63114</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D20">
         <v>15</v>
@@ -2032,343 +2063,47 @@
       <c r="F20">
         <v>2</v>
       </c>
-      <c r="G20">
-        <v>99</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>99</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J20" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" t="s">
+        <v>58</v>
       </c>
       <c r="N20">
         <v>1</v>
       </c>
       <c r="O20" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="P20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21">
-        <v>15</v>
-      </c>
-      <c r="E21">
-        <v>20</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21">
-        <v>99</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>99</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21" t="s">
-        <v>16</v>
-      </c>
-      <c r="P21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>15</v>
-      </c>
-      <c r="E22">
-        <v>20</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>99</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <v>99</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22" t="s">
-        <v>16</v>
-      </c>
-      <c r="P22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23">
-        <v>7</v>
-      </c>
-      <c r="D23">
-        <v>15</v>
-      </c>
-      <c r="E23">
-        <v>20</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <v>99</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>99</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23" t="s">
-        <v>17</v>
-      </c>
-      <c r="P23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24">
-        <v>12</v>
-      </c>
-      <c r="D24">
-        <v>15</v>
-      </c>
-      <c r="E24">
-        <v>20</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24">
-        <v>99</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>99</v>
-      </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="O24" t="s">
-        <v>16</v>
-      </c>
-      <c r="P24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25">
-        <v>13</v>
-      </c>
-      <c r="D25">
-        <v>15</v>
-      </c>
-      <c r="E25">
-        <v>20</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25">
-        <v>99</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>99</v>
-      </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25" t="s">
-        <v>16</v>
-      </c>
-      <c r="P25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26">
-        <v>17</v>
-      </c>
-      <c r="D26">
-        <v>15</v>
-      </c>
-      <c r="E26">
-        <v>20</v>
-      </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="G26">
-        <v>99</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26">
-        <v>99</v>
-      </c>
-      <c r="M26">
-        <v>1</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="O26" t="s">
-        <v>16</v>
-      </c>
-      <c r="P26" t="s">
-        <v>17</v>
+      <c r="Q20" s="1">
+        <v>62589</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:P25">
-    <sortCondition ref="A2:A25"/>
+  <sortState ref="A2:P16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B20" r:id="rId2" display="mailto:rkagorkle1@yahoo.com" xr:uid="{0A014C36-CD36-4F10-B2DD-84ECE3E12EE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>